<commit_message>
Consertando o bug da análise da produção de milho (R$)/km² com desmatamento e acrescentando gráficos comparativos
</commit_message>
<xml_diff>
--- a/Impacto-Produção de Milho(R$)-Desmatamento-Pará/Produção de Milho(R$)-km + desmatamento.xlsx
+++ b/Impacto-Produção de Milho(R$)-Desmatamento-Pará/Produção de Milho(R$)-km + desmatamento.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,10 +457,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1990</v>
+        <v>1999</v>
       </c>
       <c r="B2" t="n">
-        <v>4890</v>
+        <v>5111</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -468,15 +468,15 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>230018.6582838494</v>
+        <v>230018.66</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1991</v>
+        <v>2000</v>
       </c>
       <c r="B3" t="n">
-        <v>3780</v>
+        <v>6671</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -484,15 +484,15 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>222991.587245047</v>
+        <v>222991.59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1992</v>
+        <v>2001</v>
       </c>
       <c r="B4" t="n">
-        <v>3787</v>
+        <v>5237</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -500,15 +500,15 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>200853.9547731077</v>
+        <v>200853.95</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1993</v>
+        <v>2002</v>
       </c>
       <c r="B5" t="n">
-        <v>4284</v>
+        <v>7510</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -516,15 +516,15 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>217638.3991115586</v>
+        <v>217638.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1994</v>
+        <v>2003</v>
       </c>
       <c r="B6" t="n">
-        <v>4284</v>
+        <v>7145</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -532,15 +532,15 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>307444.8830751837</v>
+        <v>307444.88</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1995</v>
+        <v>2004</v>
       </c>
       <c r="B7" t="n">
-        <v>7845</v>
+        <v>8870</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -548,15 +548,15 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>284869.2949272274</v>
+        <v>284869.29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1996</v>
+        <v>2005</v>
       </c>
       <c r="B8" t="n">
-        <v>6135</v>
+        <v>5899</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -564,15 +564,15 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>230198.2192820561</v>
+        <v>230198.22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1997</v>
+        <v>2006</v>
       </c>
       <c r="B9" t="n">
-        <v>4139</v>
+        <v>5659</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -580,15 +580,15 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>228859.6421186697</v>
+        <v>228859.64</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1998</v>
+        <v>2007</v>
       </c>
       <c r="B10" t="n">
-        <v>5829</v>
+        <v>5526</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -596,15 +596,15 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>106208.0410469003</v>
+        <v>106208.04</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1999</v>
+        <v>2008</v>
       </c>
       <c r="B11" t="n">
-        <v>5111</v>
+        <v>5607</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -612,15 +612,15 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>107539.3528102039</v>
+        <v>107539.35</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2000</v>
+        <v>2009</v>
       </c>
       <c r="B12" t="n">
-        <v>6671</v>
+        <v>4281</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -628,15 +628,15 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>110131.0488324591</v>
+        <v>110131.05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2001</v>
+        <v>2010</v>
       </c>
       <c r="B13" t="n">
-        <v>5237</v>
+        <v>3770</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -644,15 +644,15 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>91310.94886240723</v>
+        <v>91310.95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2002</v>
+        <v>2011</v>
       </c>
       <c r="B14" t="n">
-        <v>7510</v>
+        <v>3008</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -660,15 +660,15 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>217666.9619571189</v>
+        <v>217666.96</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="B15" t="n">
-        <v>7145</v>
+        <v>1741</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -676,15 +676,15 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>211924.9067092369</v>
+        <v>211924.91</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2004</v>
+        <v>2013</v>
       </c>
       <c r="B16" t="n">
-        <v>8870</v>
+        <v>2346</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -692,15 +692,15 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>223633.627004179</v>
+        <v>223633.63</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2005</v>
+        <v>2014</v>
       </c>
       <c r="B17" t="n">
-        <v>5899</v>
+        <v>1887</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -708,15 +708,15 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>181030.2514322489</v>
+        <v>181030.25</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="B18" t="n">
-        <v>5659</v>
+        <v>2153</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -724,15 +724,15 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>213673.7591899481</v>
+        <v>213673.76</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2007</v>
+        <v>2016</v>
       </c>
       <c r="B19" t="n">
-        <v>5526</v>
+        <v>2992</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -740,15 +740,15 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>233285.9465516377</v>
+        <v>233285.95</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2008</v>
+        <v>2017</v>
       </c>
       <c r="B20" t="n">
-        <v>5607</v>
+        <v>2433</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -756,15 +756,15 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>210444.2662843391</v>
+        <v>210444.27</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2009</v>
+        <v>2018</v>
       </c>
       <c r="B21" t="n">
-        <v>4281</v>
+        <v>2744</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -772,15 +772,15 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>210989.7773499699</v>
+        <v>210989.78</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="B22" t="n">
-        <v>3770</v>
+        <v>4172</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -788,15 +788,15 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>212645.4706557688</v>
+        <v>212645.47</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2011</v>
+        <v>2020</v>
       </c>
       <c r="B23" t="n">
-        <v>3008</v>
+        <v>4899</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -804,190 +804,8 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>278020.5030253442</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>2012</v>
-      </c>
-      <c r="B24" t="n">
-        <v>1741</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>2013</v>
-      </c>
-      <c r="B25" t="n">
-        <v>2346</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>2014</v>
-      </c>
-      <c r="B26" t="n">
-        <v>1887</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>2015</v>
-      </c>
-      <c r="B27" t="n">
-        <v>2153</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>2016</v>
-      </c>
-      <c r="B28" t="n">
-        <v>2992</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>2017</v>
-      </c>
-      <c r="B29" t="n">
-        <v>2433</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>2018</v>
-      </c>
-      <c r="B30" t="n">
-        <v>2744</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>2019</v>
-      </c>
-      <c r="B31" t="n">
-        <v>4172</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B32" t="n">
-        <v>4899</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B33" t="n">
-        <v>5238</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>2022</v>
-      </c>
-      <c r="B34" t="n">
-        <v>4162</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr"/>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>2023</v>
-      </c>
-      <c r="B35" t="n">
-        <v>3299</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>2024</v>
-      </c>
-      <c r="B36" t="n">
-        <v>2362</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Pará</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
+        <v>278020.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>